<commit_message>
Set required EV sales to 0
</commit_message>
<xml_diff>
--- a/InputData/trans/BMRESP/BAU Min Req EV Sales Perc.xlsx
+++ b/InputData/trans/BMRESP/BAU Min Req EV Sales Perc.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22827"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Katelyn\Dropbox\OR EPS Input Data\OR EPS\OR InputData\trans\BMRESP\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Meghan\Dropbox (Energy Innovation)\EPS Versions\eps-1.5.0-us-wipL\InputData\trans\BMRESP\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3D69B5B-A143-488B-BB56-52892A39B278}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="60" windowWidth="23955" windowHeight="12090"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -22,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="13">
   <si>
     <t>BMRESP BAU Minimum Required EV Sales Percentage</t>
   </si>
@@ -30,7 +29,13 @@
     <t>Source:</t>
   </si>
   <si>
+    <t>none needed</t>
+  </si>
+  <si>
     <t>Notes</t>
+  </si>
+  <si>
+    <t>There is no minimum required EV sales percentage</t>
   </si>
   <si>
     <t>LDVs</t>
@@ -51,66 +56,17 @@
     <t>motorbikes</t>
   </si>
   <si>
-    <t xml:space="preserve">CARB’s most recent assessment of the ZEV program estimates automakers will need to reach less than 8 percent ZEV sales by 2025 to meet the 22 percent ZEV credit requirement. Presumably this 8% accounts for ZEV credit banking and other complexities. </t>
+    <t>in the United States for any vehicle type.</t>
   </si>
   <si>
-    <t>Oregon's 50,000 EV goal by the end of 2020 is aspirational, not mandated anywhere (likely to achieve about 35,000 by the end of 2020.) The targets in SB 1044 are also aspirational.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> https://www.ucsusa.org/resources/what-zev#.XFfVKi2ZNp8%20</t>
-  </si>
-  <si>
-    <t>https://ww2.arb.ca.gov/sites/default/files/2019-12/SB%20498%20Report%20Draft%20121719.pdf</t>
-  </si>
-  <si>
-    <t>California Air Resources Board</t>
-  </si>
-  <si>
-    <t>pg. 76</t>
-  </si>
-  <si>
-    <t>DRAFT: ASSESSMENT OF CARB’S ZERO-EMISSION VEHICLE PROGRAMS PER SENATE BILL 498</t>
-  </si>
-  <si>
-    <t>Dec 2019</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Thus, the EPS should use a </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>minimum EV portion of sales of 8% in 2025, increasing 1% per year from 0% in 2017</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> (the trajectory of the ZEV credit requirements). </t>
-    </r>
+    <t>Sales Percentage (dimensionless)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0\ ;\(&quot;$&quot;#,##0\)"/>
-    <numFmt numFmtId="165" formatCode="0.00_)"/>
-  </numFmts>
-  <fonts count="14">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -126,102 +82,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="8"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="12"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <b/>
-      <i/>
-      <sz val="16"/>
-      <name val="Helv"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color indexed="8"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="ＭＳ Ｐゴシック"/>
-      <family val="3"/>
-      <charset val="128"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="2">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="22"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="26"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="3">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -229,251 +99,19 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="double">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="105">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="2" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="10" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="10" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="10" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="10" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="10" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="10" fontId="5" fillId="3" borderId="1" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="10" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFont="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="104"/>
-    <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="105">
-    <cellStyle name="Comma 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
-    <cellStyle name="Comma 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
-    <cellStyle name="Comma 2 3" xfId="103" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
-    <cellStyle name="Comma 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
-    <cellStyle name="Comma 3 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
-    <cellStyle name="Comma 3 3" xfId="5" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
-    <cellStyle name="Comma 4" xfId="6" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
-    <cellStyle name="Comma0" xfId="7" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
-    <cellStyle name="Currency0" xfId="8" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
-    <cellStyle name="Date" xfId="9" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
-    <cellStyle name="Fixed" xfId="10" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
-    <cellStyle name="Grey" xfId="11" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
-    <cellStyle name="Heading 1 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
-    <cellStyle name="Heading 2 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
-    <cellStyle name="Hyperlink" xfId="104" builtinId="8"/>
-    <cellStyle name="Input [yellow]" xfId="14" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
-    <cellStyle name="Input [yellow] 2" xfId="15" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
-    <cellStyle name="Input [yellow] 2 2" xfId="16" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
-    <cellStyle name="Input [yellow] 2 3" xfId="17" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
-    <cellStyle name="Input [yellow] 2 4" xfId="18" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
-    <cellStyle name="Input [yellow] 2 5" xfId="19" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal - Style1" xfId="20" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
-    <cellStyle name="Normal 10" xfId="21" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
-    <cellStyle name="Normal 10 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
-    <cellStyle name="Normal 10 3" xfId="23" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
-    <cellStyle name="Normal 11" xfId="24" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
-    <cellStyle name="Normal 11 2" xfId="25" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
-    <cellStyle name="Normal 12" xfId="26" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
-    <cellStyle name="Normal 13" xfId="27" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
-    <cellStyle name="Normal 14" xfId="28" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
-    <cellStyle name="Normal 15" xfId="29" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
-    <cellStyle name="Normal 15 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
-    <cellStyle name="Normal 16" xfId="31" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
-    <cellStyle name="Normal 17" xfId="32" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
-    <cellStyle name="Normal 18" xfId="33" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
-    <cellStyle name="Normal 19" xfId="34" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
-    <cellStyle name="Normal 19 2" xfId="35" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
-    <cellStyle name="Normal 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
-    <cellStyle name="Normal 2 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
-    <cellStyle name="Normal 20" xfId="38" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
-    <cellStyle name="Normal 20 2" xfId="39" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
-    <cellStyle name="Normal 21" xfId="40" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
-    <cellStyle name="Normal 21 2" xfId="41" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
-    <cellStyle name="Normal 22" xfId="42" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
-    <cellStyle name="Normal 22 2" xfId="43" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Normal 23" xfId="44" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
-    <cellStyle name="Normal 23 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
-    <cellStyle name="Normal 24" xfId="46" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
-    <cellStyle name="Normal 24 2" xfId="47" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
-    <cellStyle name="Normal 25" xfId="48" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
-    <cellStyle name="Normal 26" xfId="49" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
-    <cellStyle name="Normal 27" xfId="50" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
-    <cellStyle name="Normal 28" xfId="51" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Normal 29" xfId="52" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
-    <cellStyle name="Normal 3" xfId="53" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
-    <cellStyle name="Normal 30" xfId="54" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
-    <cellStyle name="Normal 31" xfId="55" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
-    <cellStyle name="Normal 32" xfId="56" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
-    <cellStyle name="Normal 4" xfId="57" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
-    <cellStyle name="Normal 4 2" xfId="58" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
-    <cellStyle name="Normal 4 3" xfId="59" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
-    <cellStyle name="Normal 4 4" xfId="60" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
-    <cellStyle name="Normal 4 5" xfId="101" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
-    <cellStyle name="Normal 5" xfId="61" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
-    <cellStyle name="Normal 5 2" xfId="62" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
-    <cellStyle name="Normal 5 3" xfId="63" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
-    <cellStyle name="Normal 6" xfId="64" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
-    <cellStyle name="Normal 6 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
-    <cellStyle name="Normal 6 3" xfId="66" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
-    <cellStyle name="Normal 7" xfId="67" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
-    <cellStyle name="Normal 7 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
-    <cellStyle name="Normal 7 3" xfId="69" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
-    <cellStyle name="Normal 8" xfId="70" xr:uid="{00000000-0005-0000-0000-000048000000}"/>
-    <cellStyle name="Normal 8 2" xfId="71" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
-    <cellStyle name="Normal 8 3" xfId="72" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
-    <cellStyle name="Normal 9" xfId="73" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
-    <cellStyle name="Normal 9 2" xfId="74" xr:uid="{00000000-0005-0000-0000-00004C000000}"/>
-    <cellStyle name="Normal 9 3" xfId="75" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
-    <cellStyle name="Percent [2]" xfId="76" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
-    <cellStyle name="Percent 2" xfId="77" xr:uid="{00000000-0005-0000-0000-00004F000000}"/>
-    <cellStyle name="Percent 2 2" xfId="78" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
-    <cellStyle name="Percent 2 3" xfId="79" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
-    <cellStyle name="Percent 2 4" xfId="80" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
-    <cellStyle name="Percent 2 5" xfId="102" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
-    <cellStyle name="Percent 3" xfId="81" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
-    <cellStyle name="Percent 4" xfId="82" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
-    <cellStyle name="Percent 5" xfId="83" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
-    <cellStyle name="Percent 6" xfId="84" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
-    <cellStyle name="Percent 7" xfId="85" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
-    <cellStyle name="Percent 8" xfId="86" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
-    <cellStyle name="Percent 9" xfId="87" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
-    <cellStyle name="Standard 2" xfId="88" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
-    <cellStyle name="Total 2" xfId="89" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
-    <cellStyle name="Total 2 2" xfId="90" xr:uid="{00000000-0005-0000-0000-00005D000000}"/>
-    <cellStyle name="Total 2 3" xfId="91" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
-    <cellStyle name="Total 3" xfId="92" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
-    <cellStyle name="Total 3 2" xfId="93" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
-    <cellStyle name="Total 4" xfId="94" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
-    <cellStyle name="Total 4 2" xfId="95" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
-    <cellStyle name="Total 5" xfId="96" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
-    <cellStyle name="Total 5 2" xfId="97" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
-    <cellStyle name="Total 6" xfId="98" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
-    <cellStyle name="Total 7" xfId="99" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
-    <cellStyle name="標準_Book1" xfId="100" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -564,23 +202,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -616,23 +237,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -808,107 +412,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:10">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>13</v>
+        <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:10" s="2" customFormat="1">
-      <c r="A4" s="1"/>
-      <c r="B4" t="s">
-        <v>15</v>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A8" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" s="2" customFormat="1">
-      <c r="A5" s="1"/>
-      <c r="B5" s="4" t="s">
-        <v>16</v>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A9" t="s">
+        <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:10">
-      <c r="B6" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-    </row>
-    <row r="7" spans="1:10">
-      <c r="B7" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10">
-      <c r="B8" t="s">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
         <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10">
-      <c r="A10" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10">
-      <c r="A11" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10">
-      <c r="A13" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="2" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B7" r:id="rId1" display="https://ww2.arb.ca.gov/sites/default/files/2019-12/SB 498 Report Draft 121719.pdf" xr:uid="{3CBA5DDB-DA4E-4BCC-8700-8262E3A70919}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
   <dimension ref="A1:AJ7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
+    <col min="1" max="1" width="19.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B1">
         <v>2016</v>
       </c>
@@ -1015,9 +577,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1025,109 +587,109 @@
       <c r="C2">
         <v>0</v>
       </c>
-      <c r="D2" s="2">
-        <v>0.01</v>
-      </c>
-      <c r="E2" s="2">
-        <v>0.02</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.03</v>
-      </c>
-      <c r="G2" s="2">
-        <v>0.04</v>
-      </c>
-      <c r="H2" s="2">
-        <v>0.05</v>
-      </c>
-      <c r="I2" s="2">
-        <v>0.06</v>
-      </c>
-      <c r="J2" s="2">
-        <v>7.0000000000000007E-2</v>
-      </c>
-      <c r="K2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="L2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="M2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="N2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="O2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="P2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="Q2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="R2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="S2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="T2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="U2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="V2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="W2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="X2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="Y2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="Z2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="AA2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="AB2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="AC2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="AD2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="AE2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="AF2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="AG2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="AH2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="AI2" s="2">
-        <v>0.08</v>
-      </c>
-      <c r="AJ2" s="2">
-        <v>0.08</v>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+      <c r="G2">
+        <v>0</v>
+      </c>
+      <c r="H2">
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
+      <c r="R2">
+        <v>0</v>
+      </c>
+      <c r="S2">
+        <v>0</v>
+      </c>
+      <c r="T2">
+        <v>0</v>
+      </c>
+      <c r="U2">
+        <v>0</v>
+      </c>
+      <c r="V2">
+        <v>0</v>
+      </c>
+      <c r="W2">
+        <v>0</v>
+      </c>
+      <c r="X2">
+        <v>0</v>
+      </c>
+      <c r="Y2">
+        <v>0</v>
+      </c>
+      <c r="Z2">
+        <v>0</v>
+      </c>
+      <c r="AA2">
+        <v>0</v>
+      </c>
+      <c r="AB2">
+        <v>0</v>
+      </c>
+      <c r="AC2">
+        <v>0</v>
+      </c>
+      <c r="AD2">
+        <v>0</v>
+      </c>
+      <c r="AE2">
+        <v>0</v>
+      </c>
+      <c r="AF2">
+        <v>0</v>
+      </c>
+      <c r="AG2">
+        <v>0</v>
+      </c>
+      <c r="AH2">
+        <v>0</v>
+      </c>
+      <c r="AI2">
+        <v>0</v>
+      </c>
+      <c r="AJ2">
+        <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -1235,44 +797,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0</v>
       </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0</v>
-      </c>
-      <c r="H4" s="2">
-        <v>0</v>
-      </c>
-      <c r="I4" s="2">
-        <v>0</v>
-      </c>
-      <c r="J4" s="2">
-        <v>0</v>
-      </c>
-      <c r="K4" s="2">
-        <v>0</v>
-      </c>
-      <c r="L4" s="2">
-        <v>0</v>
-      </c>
-      <c r="M4" s="2">
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4">
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="L4">
+        <v>0</v>
+      </c>
+      <c r="M4">
         <v>0</v>
       </c>
       <c r="N4">
@@ -1345,44 +907,44 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>0</v>
       </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
-      <c r="H5" s="2">
-        <v>0</v>
-      </c>
-      <c r="I5" s="2">
-        <v>0</v>
-      </c>
-      <c r="J5" s="2">
-        <v>0</v>
-      </c>
-      <c r="K5" s="2">
-        <v>0</v>
-      </c>
-      <c r="L5" s="2">
-        <v>0</v>
-      </c>
-      <c r="M5" s="2">
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <v>0</v>
+      </c>
+      <c r="L5">
+        <v>0</v>
+      </c>
+      <c r="M5">
         <v>0</v>
       </c>
       <c r="N5">
@@ -1455,9 +1017,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -1565,9 +1127,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>0</v>
@@ -1681,7 +1243,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <tabColor theme="3"/>
   </sheetPr>
@@ -1689,12 +1251,15 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="19.26953125" customWidth="1"/>
+    <col min="1" max="1" width="19.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:36" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="2" t="s">
+        <v>12</v>
+      </c>
       <c r="B1">
         <v>2016</v>
       </c>
@@ -1801,9 +1366,9 @@
         <v>2050</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -1911,9 +1476,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -2021,9 +1586,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B4">
         <v>0</v>
@@ -2131,9 +1696,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -2241,9 +1806,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B6">
         <v>0</v>
@@ -2351,9 +1916,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:36" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B7">
         <v>0</v>

</xml_diff>